<commit_message>
Update the MAC address spreadsheet
</commit_message>
<xml_diff>
--- a/speedtracker_macs.xlsx
+++ b/speedtracker_macs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a96234ccd6220a93/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\repos\st_pitweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41007714-6F82-4D7E-AD8F-9C8A869B2EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC8B444-A395-46F8-8737-6FCD000005B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="8745" windowWidth="16200" windowHeight="9315" xr2:uid="{ED44B6A6-3786-41EF-BFD5-7B936235A880}"/>
+    <workbookView xWindow="32775" yWindow="11355" windowWidth="9480" windowHeight="12240" xr2:uid="{ED44B6A6-3786-41EF-BFD5-7B936235A880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>MAC Address</t>
   </si>
@@ -108,6 +108,72 @@
   </si>
   <si>
     <t>74:4D:BD:88:D2:98</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D4:68</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:68:C4</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:CE:C0</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:CE:DC</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D0:C8</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:69:A4</t>
+  </si>
+  <si>
+    <t>REPAIR</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D0:60</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D3:40</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:69:D8</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:CE:3C</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D1:70</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:CF:04</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:CE:B4</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:6A:8C</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D2:6C</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:6A:14</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D4:78</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D1:A8</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D1:FC</t>
+  </si>
+  <si>
+    <t>80:65:99:A1:68:88</t>
+  </si>
+  <si>
+    <t>74:4D:BD:88:D1:38</t>
   </si>
 </sst>
 </file>
@@ -157,13 +223,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,19 +573,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A9EEFB-2DCA-4807-B7C0-125E3A367E53}">
   <dimension ref="E4:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="44" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -524,7 +596,7 @@
       </c>
     </row>
     <row r="5" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -535,7 +607,7 @@
       </c>
     </row>
     <row r="6" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -546,7 +618,7 @@
       </c>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -557,7 +629,7 @@
       </c>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -568,7 +640,7 @@
       </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -579,7 +651,7 @@
       </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="2">
+      <c r="E10" s="4">
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -590,7 +662,7 @@
       </c>
     </row>
     <row r="11" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -601,7 +673,7 @@
       </c>
     </row>
     <row r="12" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -612,7 +684,7 @@
       </c>
     </row>
     <row r="13" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -623,7 +695,7 @@
       </c>
     </row>
     <row r="14" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -634,7 +706,7 @@
       </c>
     </row>
     <row r="15" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="2">
+      <c r="E15" s="4">
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -645,7 +717,7 @@
       </c>
     </row>
     <row r="16" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -656,7 +728,7 @@
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2">
+      <c r="E17" s="4">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -667,7 +739,7 @@
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2">
+      <c r="E18" s="4">
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -678,7 +750,7 @@
       </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="2">
+      <c r="E19" s="4">
         <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -689,7 +761,7 @@
       </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="2">
+      <c r="E20" s="4">
         <v>16</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -700,284 +772,428 @@
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
+      <c r="E21" s="4">
         <v>17</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="2">
+      <c r="E22" s="4">
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="2">
+      <c r="E23" s="4">
         <v>19</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="2">
+      <c r="E24" s="4">
         <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
+      <c r="E25" s="4">
         <v>21</v>
       </c>
+      <c r="F25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="2">
+      <c r="E26" s="4">
         <v>22</v>
       </c>
+      <c r="F26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="2">
+      <c r="E27" s="4">
         <v>23</v>
       </c>
+      <c r="F27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="2">
+      <c r="E28" s="4">
         <v>24</v>
       </c>
+      <c r="F28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="2">
+      <c r="E29" s="4">
         <v>25</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="2">
+      <c r="E30" s="4">
         <v>26</v>
       </c>
+      <c r="F30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="2">
+      <c r="E31" s="4">
         <v>27</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="2">
+      <c r="E32" s="4">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="2">
+      <c r="F32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="2">
+      <c r="F33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="2">
+      <c r="F34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="2">
+      <c r="F35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="4">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="2">
+      <c r="F36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="4">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="2">
+      <c r="F37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="4">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="2">
+      <c r="F38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="2">
+      <c r="F39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="2">
+      <c r="F40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="2">
+      <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="2">
+      <c r="F42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="4">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="2">
+      <c r="F43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="2">
+      <c r="F44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="4">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="2">
+      <c r="F45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="4">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="2">
+      <c r="F46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="2">
+    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="4">
         <v>44</v>
       </c>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="2">
+      <c r="E49" s="4">
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="2">
+      <c r="E50" s="4">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="2">
+      <c r="E51" s="4">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="2">
+      <c r="E52" s="4">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="2">
+      <c r="E53" s="4">
         <v>49</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="2">
+      <c r="E54" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="2">
+      <c r="E55" s="4">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="2">
+      <c r="E56" s="4">
         <v>52</v>
       </c>
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="2">
+      <c r="E57" s="4">
         <v>53</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="2">
+      <c r="E58" s="4">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="2">
+      <c r="E59" s="4">
         <v>55</v>
       </c>
     </row>
     <row r="60" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="2">
+      <c r="E60" s="4">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="2">
+      <c r="E61" s="4">
         <v>57</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="2">
+      <c r="E62" s="4">
         <v>58</v>
       </c>
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="2">
+      <c r="E63" s="4">
         <v>59</v>
       </c>
     </row>
     <row r="64" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="2">
+      <c r="E64" s="4">
         <v>60</v>
       </c>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="2">
+      <c r="E65" s="4">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="2">
+      <c r="E66" s="4">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="2">
+      <c r="E67" s="4">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="2">
+      <c r="E68" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="2">
+      <c r="E69" s="4">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="2">
+      <c r="E70" s="4">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="2">
+      <c r="E71" s="4">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" s="2">
+      <c r="E72" s="4">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="2">
+      <c r="E73" s="4">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="2">
+      <c r="E74" s="4">
         <v>70</v>
       </c>
     </row>

</xml_diff>